<commit_message>
upload of synthetic case
frontiers in Water
</commit_message>
<xml_diff>
--- a/Data/InvestmentModule_ex.xlsx
+++ b/Data/InvestmentModule_ex.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapy\OneDrive - COWI\Scripts\Main_model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cowi-my.sharepoint.com/personal/rapy_cowi_com/Documents/WHATIF/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="206" documentId="10_ncr:100000_{D7D8820F-DB18-4DDB-822F-8CBD99F1944D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D4BD72DD-6A5A-4BE4-98B5-BA2D379A8956}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{A0350182-FDE0-4E54-A0DC-2825D8DE370D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CCDC99A7-7F43-4508-8CA4-C5D366D19F6B}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2760" windowWidth="14790" windowHeight="10320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
     <sheet name="Investments" sheetId="2" r:id="rId2"/>
-    <sheet name="InvestmentPhases" sheetId="4" r:id="rId3"/>
+    <sheet name="InvestYear" sheetId="5" r:id="rId3"/>
+    <sheet name="InvestmentPhases" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="110">
   <si>
     <t>#HydroPower Plants</t>
   </si>
@@ -125,9 +128,6 @@
     <t>#Investment phase</t>
   </si>
   <si>
-    <t>ip2</t>
-  </si>
-  <si>
     <t>ninvphase</t>
   </si>
   <si>
@@ -203,26 +203,176 @@
     <t>#Fix operational costs</t>
   </si>
   <si>
-    <t>Investment types: hydro, reservoir, transfer, transmission, power, farming</t>
-  </si>
-  <si>
     <t>farming</t>
   </si>
   <si>
     <t>iMaxInv</t>
   </si>
   <si>
-    <t>LionTurbine</t>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>Biofuels</t>
+  </si>
+  <si>
+    <t>inv_year</t>
+  </si>
+  <si>
+    <t>TheDam</t>
+  </si>
+  <si>
+    <t>Desalinization</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>sInvest</t>
+  </si>
+  <si>
+    <t>nexus</t>
+  </si>
+  <si>
+    <t>ag</t>
+  </si>
+  <si>
+    <t>eg</t>
+  </si>
+  <si>
+    <t>NewSolar</t>
+  </si>
+  <si>
+    <t>NewTurbine</t>
+  </si>
+  <si>
+    <t>reservoir</t>
+  </si>
+  <si>
+    <t>wa</t>
+  </si>
+  <si>
+    <t>NewRainfed</t>
+  </si>
+  <si>
+    <t>NewIrrigated</t>
+  </si>
+  <si>
+    <t>sInvYear</t>
+  </si>
+  <si>
+    <t>InvestYear</t>
+  </si>
+  <si>
+    <t>NewWind</t>
+  </si>
+  <si>
+    <t>IrrigEfficiency</t>
   </si>
   <si>
     <t>PantherFarm</t>
+  </si>
+  <si>
+    <t>NexusPlan</t>
+  </si>
+  <si>
+    <t>SiloPlan</t>
+  </si>
+  <si>
+    <t>noinvest</t>
+  </si>
+  <si>
+    <t>NexusPlan2</t>
+  </si>
+  <si>
+    <t>SiloPlan2</t>
+  </si>
+  <si>
+    <t>inv_max</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>BasePlan</t>
+  </si>
+  <si>
+    <t>REM: iInvType not used except in custom "WHATIF_montecarlo.py"</t>
+  </si>
+  <si>
+    <t>Potential investments should be entered both: here and in the corresponding data sheet (e.g. hydropower in hydropower data, irrigation in agriculture data, etc …)</t>
+  </si>
+  <si>
+    <t>In this sheet describe the investment capital costs (iCAPEX), FIX operational costs (iFixOPEX) - other costs are in the specific data sheets, construction time (iConstTime)</t>
+  </si>
+  <si>
+    <t>lifetime (iLifeTime), capacity (iInvCap) in the unit of the corresponding capacity</t>
+  </si>
+  <si>
+    <t>All other technical parameters depend on the investment type and need to be filled in the respective data sheet, while setting the capacity to 0 !</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraints can be defined: inv_replace defines which of the infrastructure the investment replaces (of the same type - e.g. irrigation replacing rainfed), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inv_after forces the investment to be available only after another investment has been selected, inv_group bounds to investments that have to be selected simulteanously </t>
+  </si>
+  <si>
+    <t>inv_max: is only active if option Investment module is "continuous": "binary" means that  the investment decision to be binary (0 or 1=100%), any number, fraction limits to scale the investment (1= max 100%, 1.5=max 150%,  2= max 200%, etc …)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#maximum investment scaling </t>
+  </si>
+  <si>
+    <t>(-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hard coded: "binary" in inv_max forces the investment decision to be binary (0 or 1=100%) - this is the default case if "Investment module" option is =1 </t>
+  </si>
+  <si>
+    <t>The iInvYear parameter forces the model to select an investment at a specific investment phase</t>
+  </si>
+  <si>
+    <t>Leave blank tolet investment decision to the objective function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define investment phases </t>
+  </si>
+  <si>
+    <t># Forces to invest at a given investment phase</t>
+  </si>
+  <si>
+    <t>units: (-)</t>
+  </si>
+  <si>
+    <t>1 means 100% of the investment is developed, any share (e.g. 0.5) will lead to a partial investment</t>
+  </si>
+  <si>
+    <t>Columns are investment phases, lines are potential investments</t>
+  </si>
+  <si>
+    <t>Investment phases occur at specific time steps (invphase_t)</t>
+  </si>
+  <si>
+    <t>Investment phases represent that decisions are not taken continuously but at specific time intervals (e.g. every 5 years)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It also enables to considerably reduce computing requierments ! </t>
+  </si>
+  <si>
+    <t>Binary investments are costly ad defining many investment phases with multiple potential investments will increase considerably computing time</t>
+  </si>
+  <si>
+    <t>Investment phases have budget constraints (iMaxInv), this will limit the total investment costs within the investment phase</t>
+  </si>
+  <si>
+    <t>Leftover budget from previous investment phases can be used in current investment phase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -273,18 +423,29 @@
     </font>
     <font>
       <sz val="9"/>
-      <color theme="10"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
-      <color indexed="8"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,13 +466,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,7 +588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -454,21 +633,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -719,43 +903,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -772,7 +956,7 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -784,13 +968,13 @@
         <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="8">
         <v>1</v>
       </c>
@@ -806,19 +990,22 @@
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
       <c r="J7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -827,6 +1014,32 @@
         <v>1</v>
       </c>
       <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9">
         <v>1</v>
       </c>
     </row>
@@ -837,321 +1050,322 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="22.08984375" customWidth="1"/>
-    <col min="2" max="6" width="13.36328125" customWidth="1"/>
-    <col min="7" max="7" width="15.90625" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" customWidth="1"/>
-    <col min="9" max="9" width="12.08984375" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" customWidth="1"/>
-    <col min="12" max="12" width="14.6328125" customWidth="1"/>
+    <col min="2" max="2" width="18.875" customWidth="1"/>
+    <col min="3" max="7" width="13.375" customWidth="1"/>
+    <col min="8" max="8" width="15.875" customWidth="1"/>
+    <col min="9" max="9" width="13.75" customWidth="1"/>
+    <col min="10" max="10" width="12.125" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:11" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="13"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
-      <c r="I1" s="12"/>
+      <c r="I1" s="13"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="F2" s="13"/>
+      <c r="E2" s="2"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
-      <c r="I2" s="12"/>
+      <c r="I2" s="13"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="13"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="12"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="15"/>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B4" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="14"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="16"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B5" s="18"/>
       <c r="C5" s="19"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="5"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B6" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="C6" s="5"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="5"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="20"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F7" s="20"/>
-      <c r="G7" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="20"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="20"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
       <c r="C8" s="22"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B10" s="38" t="s">
+        <v>91</v>
+      </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="23"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B11" s="38" t="s">
+        <v>92</v>
+      </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="20"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="21"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B12" s="38" t="s">
+        <v>93</v>
+      </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B13" s="8"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B14" s="25"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="20"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="23"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B16" s="38" t="s">
+        <v>86</v>
+      </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="23"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B17" s="39" t="s">
+        <v>96</v>
+      </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="23"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="30"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" ht="69" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="D21" s="9" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>2</v>
+      <c r="H21" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>2</v>
@@ -1159,93 +1373,555 @@
       <c r="J21" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="K21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="H22" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="I22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="32">
-        <v>150</v>
-      </c>
-      <c r="C23" s="32">
-        <v>5</v>
-      </c>
-      <c r="D23" s="33">
-        <v>1</v>
-      </c>
-      <c r="E23" s="8">
-        <f t="shared" ref="E23" si="0">50*12</f>
-        <v>600</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="34">
-        <v>500</v>
-      </c>
-      <c r="H23" s="7"/>
+      <c r="K22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="30">
+        <v>15</v>
+      </c>
+      <c r="D23" s="30">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8">
+        <v>48</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="7">
+        <v>30</v>
+      </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
-      <c r="K23" s="38"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
+      <c r="K23" s="7"/>
+      <c r="L23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B24" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="30">
+        <v>7</v>
+      </c>
+      <c r="D24" s="30">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="8">
+        <v>48</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="7">
+        <v>10</v>
+      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B25" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="30">
+        <v>20</v>
+      </c>
+      <c r="D25" s="30">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8">
+        <v>48</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="31">
+        <v>40</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B26" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="30">
+        <v>12</v>
+      </c>
+      <c r="D26" s="30">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0</v>
+      </c>
+      <c r="F26" s="8">
+        <v>48</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="31">
+        <v>200</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B27" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="30">
+        <v>8</v>
+      </c>
+      <c r="D27" s="30">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8">
+        <v>48</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" s="31">
+        <v>200</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B28" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="8">
+        <v>48</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="7">
+        <v>2</v>
+      </c>
+      <c r="I28" s="7"/>
+      <c r="L28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B29" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="30">
+        <v>4</v>
+      </c>
+      <c r="D29" s="30">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0</v>
+      </c>
+      <c r="F29" s="8">
+        <v>48</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29">
+        <v>15</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B30" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="30">
+        <v>5</v>
+      </c>
+      <c r="D30" s="30">
+        <v>0</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0</v>
+      </c>
+      <c r="F30" s="8">
+        <v>48</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30">
+        <v>15</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B31" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="30">
+        <v>4</v>
+      </c>
+      <c r="D31" s="30">
+        <v>0</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0</v>
+      </c>
+      <c r="F31" s="7">
+        <v>48</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31">
+        <v>20</v>
+      </c>
+      <c r="I31" t="s">
+        <v>77</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="32">
-        <v>100</v>
-      </c>
-      <c r="C24" s="32">
+      <c r="C32" s="30">
+        <v>15</v>
+      </c>
+      <c r="D32" s="30">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="8">
+        <v>48</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H32" s="7">
+        <v>30</v>
+      </c>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B33" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="30">
+        <v>7</v>
+      </c>
+      <c r="D33" s="30">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="8">
+        <v>48</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="7">
+        <v>10</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B34" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="30">
+        <v>20</v>
+      </c>
+      <c r="D34" s="30">
+        <v>0</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0</v>
+      </c>
+      <c r="F34" s="8">
+        <v>48</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="31">
+        <v>40</v>
+      </c>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="30">
+        <v>12</v>
+      </c>
+      <c r="D35" s="30">
+        <v>0</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0</v>
+      </c>
+      <c r="F35" s="8">
+        <v>48</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H35" s="31">
+        <v>200</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B36" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="30">
+        <v>8</v>
+      </c>
+      <c r="D36" s="30">
+        <v>0</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0</v>
+      </c>
+      <c r="F36" s="8">
+        <v>48</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H36" s="31">
+        <v>200</v>
+      </c>
+      <c r="I36" s="7"/>
+      <c r="L36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B37" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" s="8">
+        <v>48</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" s="7">
+        <v>2</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="L37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="30">
+        <v>4</v>
+      </c>
+      <c r="D38" s="30">
+        <v>0</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0</v>
+      </c>
+      <c r="F38" s="8">
+        <v>48</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H38">
+        <v>15</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B39" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="30">
         <v>5</v>
       </c>
-      <c r="D24" s="7">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>240</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="21">
-        <v>200</v>
-      </c>
-      <c r="H24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="38"/>
+      <c r="D39" s="30">
+        <v>0</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0</v>
+      </c>
+      <c r="F39" s="8">
+        <v>48</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39">
+        <v>15</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B40" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="30">
+        <v>4</v>
+      </c>
+      <c r="D40" s="30">
+        <v>0</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0</v>
+      </c>
+      <c r="F40" s="7">
+        <v>48</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H40">
+        <v>20</v>
+      </c>
+      <c r="I40" t="s">
+        <v>77</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1254,85 +1930,962 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A388D95A-1F22-4BA9-8CBA-1D7021C3B249}">
+  <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.90625" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="19.25" customWidth="1"/>
+    <col min="3" max="3" width="20.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B3" s="2"/>
+      <c r="C3" s="12"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B5" s="18"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B6" s="13"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B9" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B10" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B14" s="8"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="33"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B24" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="33"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B25" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="33"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B26" s="32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B27" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="33"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B28" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="33"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B29" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B30" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B31" s="36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B33" s="34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B34" s="34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B36" s="32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B37" s="35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B39" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B40" s="36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B42" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B43" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B44" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B45" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B46" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B47" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B48" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B49" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B51" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B52" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B53" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B54" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B55" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B56" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B57" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B58" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B60" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B61" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B62" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B63" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B64" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B65" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B66" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B67" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B69" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B70" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B71" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C71">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B72" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B73" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B74" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B75" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B76" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B78" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B79" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B80" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C80">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B81" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C81">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B82" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B83" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B84" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C84">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B85" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C85">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B87" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B88" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B89" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C89">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B90" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B91" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B92" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B93" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C93">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B94" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="14.25" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="46" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="18"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="8">
-        <v>200</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="8">
-        <v>100</v>
-      </c>
-      <c r="C8" s="7">
-        <f>C7+12</f>
-        <v>13</v>
+      <c r="B23" s="8">
+        <v>999</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
master to example case
</commit_message>
<xml_diff>
--- a/Data/InvestmentModule_ex.xlsx
+++ b/Data/InvestmentModule_ex.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapy\OneDrive - COWI\Scripts\Main_model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cowi-my.sharepoint.com/personal/rapy_cowi_com/Documents/WHATIF/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="206" documentId="10_ncr:100000_{D7D8820F-DB18-4DDB-822F-8CBD99F1944D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D4BD72DD-6A5A-4BE4-98B5-BA2D379A8956}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{A0350182-FDE0-4E54-A0DC-2825D8DE370D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B2C8EB20-E4AC-4CC1-82B8-D151647C0738}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2760" windowWidth="14790" windowHeight="10320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
     <sheet name="Investments" sheetId="2" r:id="rId2"/>
-    <sheet name="InvestmentPhases" sheetId="4" r:id="rId3"/>
+    <sheet name="InvestYear" sheetId="5" r:id="rId3"/>
+    <sheet name="InvestmentPhases" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
   <si>
     <t>#HydroPower Plants</t>
   </si>
@@ -125,9 +128,6 @@
     <t>#Investment phase</t>
   </si>
   <si>
-    <t>ip2</t>
-  </si>
-  <si>
     <t>ninvphase</t>
   </si>
   <si>
@@ -203,26 +203,140 @@
     <t>#Fix operational costs</t>
   </si>
   <si>
-    <t>Investment types: hydro, reservoir, transfer, transmission, power, farming</t>
-  </si>
-  <si>
     <t>farming</t>
   </si>
   <si>
     <t>iMaxInv</t>
   </si>
   <si>
-    <t>LionTurbine</t>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>Biofuels</t>
+  </si>
+  <si>
+    <t>inv_year</t>
+  </si>
+  <si>
+    <t>TheDam</t>
+  </si>
+  <si>
+    <t>Desalinization</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>NewSolar</t>
+  </si>
+  <si>
+    <t>NewTurbine</t>
+  </si>
+  <si>
+    <t>reservoir</t>
+  </si>
+  <si>
+    <t>NewRainfed</t>
+  </si>
+  <si>
+    <t>NewIrrigated</t>
+  </si>
+  <si>
+    <t>InvestYear</t>
+  </si>
+  <si>
+    <t>NewWind</t>
+  </si>
+  <si>
+    <t>IrrigEfficiency</t>
   </si>
   <si>
     <t>PantherFarm</t>
+  </si>
+  <si>
+    <t>inv_max</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>REM: iInvType not used except in custom "WHATIF_montecarlo.py"</t>
+  </si>
+  <si>
+    <t>Potential investments should be entered both: here and in the corresponding data sheet (e.g. hydropower in hydropower data, irrigation in agriculture data, etc …)</t>
+  </si>
+  <si>
+    <t>In this sheet describe the investment capital costs (iCAPEX), FIX operational costs (iFixOPEX) - other costs are in the specific data sheets, construction time (iConstTime)</t>
+  </si>
+  <si>
+    <t>lifetime (iLifeTime), capacity (iInvCap) in the unit of the corresponding capacity</t>
+  </si>
+  <si>
+    <t>All other technical parameters depend on the investment type and need to be filled in the respective data sheet, while setting the capacity to 0 !</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraints can be defined: inv_replace defines which of the infrastructure the investment replaces (of the same type - e.g. irrigation replacing rainfed), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inv_after forces the investment to be available only after another investment has been selected, inv_group bounds to investments that have to be selected simulteanously </t>
+  </si>
+  <si>
+    <t>inv_max: is only active if option Investment module is "continuous": "binary" means that  the investment decision to be binary (0 or 1=100%), any number, fraction limits to scale the investment (1= max 100%, 1.5=max 150%,  2= max 200%, etc …)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#maximum investment scaling </t>
+  </si>
+  <si>
+    <t>(-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hard coded: "binary" in inv_max forces the investment decision to be binary (0 or 1=100%) - this is the default case if "Investment module" option is =1 </t>
+  </si>
+  <si>
+    <t>The iInvYear parameter forces the model to select an investment at a specific investment phase</t>
+  </si>
+  <si>
+    <t>Leave blank tolet investment decision to the objective function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define investment phases </t>
+  </si>
+  <si>
+    <t># Forces to invest at a given investment phase</t>
+  </si>
+  <si>
+    <t>units: (-)</t>
+  </si>
+  <si>
+    <t>1 means 100% of the investment is developed, any share (e.g. 0.5) will lead to a partial investment</t>
+  </si>
+  <si>
+    <t>Columns are investment phases, lines are potential investments</t>
+  </si>
+  <si>
+    <t>Investment phases occur at specific time steps (invphase_t)</t>
+  </si>
+  <si>
+    <t>Investment phases represent that decisions are not taken continuously but at specific time intervals (e.g. every 5 years)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It also enables to considerably reduce computing requierments ! </t>
+  </si>
+  <si>
+    <t>Binary investments are costly ad defining many investment phases with multiple potential investments will increase considerably computing time</t>
+  </si>
+  <si>
+    <t>Investment phases have budget constraints (iMaxInv), this will limit the total investment costs within the investment phase</t>
+  </si>
+  <si>
+    <t>Leftover budget from previous investment phases can be used in current investment phase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -273,18 +387,29 @@
     </font>
     <font>
       <sz val="9"/>
-      <color theme="10"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
-      <color indexed="8"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,13 +430,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -454,21 +597,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -719,43 +867,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -772,7 +920,7 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -784,13 +932,13 @@
         <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="8">
         <v>1</v>
       </c>
@@ -810,15 +958,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -827,6 +975,29 @@
         <v>1</v>
       </c>
       <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9">
         <v>1</v>
       </c>
     </row>
@@ -837,25 +1008,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="22.08984375" customWidth="1"/>
-    <col min="2" max="6" width="13.36328125" customWidth="1"/>
-    <col min="7" max="7" width="15.90625" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" customWidth="1"/>
-    <col min="9" max="9" width="12.08984375" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" customWidth="1"/>
-    <col min="12" max="12" width="14.6328125" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="6" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="8" max="8" width="13.75" customWidth="1"/>
+    <col min="9" max="9" width="12.125" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -868,9 +1038,8 @@
       <c r="H1" s="13"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -882,9 +1051,8 @@
       <c r="H2" s="13"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -895,11 +1063,10 @@
       <c r="H3" s="13"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -907,14 +1074,13 @@
       <c r="E4" s="15"/>
       <c r="F4" s="16"/>
       <c r="G4" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="16"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -925,10 +1091,11 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="F6" s="20"/>
@@ -936,17 +1103,21 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="20"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
       <c r="F7" s="20"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="20"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="7"/>
@@ -956,11 +1127,10 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
-        <v>56</v>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>78</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -969,12 +1139,13 @@
       <c r="F9" s="20"/>
       <c r="G9" s="23"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10" s="38" t="s">
+        <v>79</v>
+      </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -984,9 +1155,11 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="38" t="s">
+        <v>80</v>
+      </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -996,9 +1169,11 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="20"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A12" s="38" t="s">
+        <v>81</v>
+      </c>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -1008,9 +1183,8 @@
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="8"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -1021,22 +1195,20 @@
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A14" s="25"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
-      <c r="E14" s="28"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="20"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="20"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1047,10 +1219,11 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A16" s="38" t="s">
+        <v>74</v>
+      </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1060,10 +1233,11 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A17" s="39" t="s">
+        <v>84</v>
+      </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1073,22 +1247,20 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="30"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1096,21 +1268,21 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="69" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>19</v>
@@ -1119,24 +1291,27 @@
         <v>25</v>
       </c>
       <c r="H20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="J20" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>16</v>
@@ -1148,7 +1323,7 @@
         <v>20</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>2</v>
@@ -1159,22 +1334,25 @@
       <c r="J21" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="D22" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>21</v>
@@ -1183,69 +1361,265 @@
         <v>18</v>
       </c>
       <c r="H22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="J22" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="32">
-        <v>150</v>
-      </c>
-      <c r="C23" s="32">
-        <v>5</v>
-      </c>
-      <c r="D23" s="33">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A23" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="30">
+        <v>15</v>
+      </c>
+      <c r="C23" s="30">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
       </c>
       <c r="E23" s="8">
-        <f t="shared" ref="E23" si="0">50*12</f>
-        <v>600</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="34">
-        <v>500</v>
+        <v>48</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="7">
+        <v>30</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
-      <c r="K23" s="38"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="32">
-        <v>100</v>
-      </c>
-      <c r="C24" s="32">
-        <v>5</v>
-      </c>
-      <c r="D24" s="7">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>240</v>
+      <c r="K23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A24" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="30">
+        <v>7</v>
+      </c>
+      <c r="C24" s="30">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8">
+        <v>48</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="7">
+        <v>10</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A25" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="30">
+        <v>20</v>
+      </c>
+      <c r="C25" s="30">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0</v>
+      </c>
+      <c r="E25" s="8">
+        <v>48</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="31">
+        <v>40</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A26" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="30">
+        <v>12</v>
+      </c>
+      <c r="C26" s="30">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8">
+        <v>48</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="31">
         <v>200</v>
       </c>
-      <c r="H24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="38"/>
+      <c r="K26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A27" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="30">
+        <v>8</v>
+      </c>
+      <c r="C27" s="30">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0</v>
+      </c>
+      <c r="E27" s="8">
+        <v>48</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="31">
+        <v>200</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A28" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" s="8">
+        <v>48</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="7">
+        <v>2</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="K28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A29" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="30">
+        <v>4</v>
+      </c>
+      <c r="C29" s="30">
+        <v>0</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0</v>
+      </c>
+      <c r="E29" s="8">
+        <v>48</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29">
+        <v>15</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A30" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="30">
+        <v>5</v>
+      </c>
+      <c r="C30" s="30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0</v>
+      </c>
+      <c r="E30" s="8">
+        <v>48</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30">
+        <v>15</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A31" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="30">
+        <v>4</v>
+      </c>
+      <c r="C31" s="30">
+        <v>0</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0</v>
+      </c>
+      <c r="E31" s="7">
+        <v>48</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31">
+        <v>20</v>
+      </c>
+      <c r="H31" t="s">
+        <v>71</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1254,85 +1628,454 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A388D95A-1F22-4BA9-8CBA-1D7021C3B249}">
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.90625" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="20.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="2"/>
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="18"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="13"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="33"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="33"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="33"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="33"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="33"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="14.25" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="46" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="18"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="8">
+        <v>999</v>
+      </c>
+      <c r="C23" s="8">
         <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="8">
-        <v>200</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="8">
-        <v>100</v>
-      </c>
-      <c r="C8" s="7">
-        <f>C7+12</f>
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>